<commit_message>
Fix the issue with the glueStreaming parameter. GLUE_TYPE is gluestreaming. Updated CQLReplicator-calculator.xlsx
</commit_message>
<xml_diff>
--- a/glue/resources/CQLReplicator-calculator.xlsx
+++ b/glue/resources/CQLReplicator-calculator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kolesnn/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kolesnn/IdeaProjects/cql-replicator/glue/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF3E4AA-900C-6D42-A811-4B44094D5670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BD74EB-2F44-9142-9D5E-D7C12DEAF3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17800" xr2:uid="{E1F5BCB3-0904-F044-A203-C0CE43AF672C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="58380" windowHeight="25260" xr2:uid="{E1F5BCB3-0904-F044-A203-C0CE43AF672C}"/>
   </bookViews>
   <sheets>
     <sheet name="List of artifacts" sheetId="1" r:id="rId1"/>
@@ -760,7 +760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B84072-A83D-2743-8F9D-667BA63B4BA7}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -864,8 +864,8 @@
 }' --orw 8000000</v>
       </c>
       <c r="F2" s="5">
-        <f>IF(H2="G.025X",750,IF(H2="G.1X",1500,3000)) * O2</f>
-        <v>178875</v>
+        <f>IF(H2="G.025X",350,IF(H2="G.1X",1400,2800)) * O2</f>
+        <v>83475</v>
       </c>
       <c r="G2" s="5">
         <f>(ROUND(B2/Parameters!B$15, 0) + 1)</f>
@@ -906,7 +906,7 @@
       </c>
       <c r="Q2" s="8">
         <f>ROUNDUP(((C2 * 1024 * 1024) / F2) / 3600, 0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R2" s="8">
         <f>IF(H2 = "G.025X", 8000000, IF(H2= "G.1X", 16000000, IF(H2= "G.2X", 32000000)))</f>
@@ -939,8 +939,8 @@
 }' --orw 8000000</v>
       </c>
       <c r="F3" s="5">
-        <f t="shared" ref="F3:F6" si="1">IF(H3="G.025X",750,IF(H3="G.1X",1500,3000)) * O3</f>
-        <v>67500</v>
+        <f t="shared" ref="F3:F6" si="1">IF(H3="G.025X",350,IF(H3="G.1X",1400,2800)) * O3</f>
+        <v>31500</v>
       </c>
       <c r="G3" s="5">
         <f>(ROUND(B3/Parameters!B$15, 0) + 1)</f>
@@ -981,7 +981,7 @@
       </c>
       <c r="Q3" s="8">
         <f>ROUNDUP(((C3 * 1024 * 1024) / F3) / 3600, 0)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R3" s="8">
         <f t="shared" ref="R3:R6" si="7">IF(H3 = "G.025X", 8000000, IF(H3= "G.1X", 16000000, IF(H3= "G.2X", 32000000)))</f>
@@ -1015,7 +1015,7 @@
       </c>
       <c r="F4" s="5">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>2800</v>
       </c>
       <c r="G4" s="5">
         <f>(ROUND(B4/Parameters!B$15, 0) + 1)</f>
@@ -1089,15 +1089,15 @@
 }' --orw 16000000</v>
       </c>
       <c r="F5" s="5">
-        <f t="shared" ref="F5" si="9">IF(H5="G.025X",750,IF(H5="G.1X",1500,3000)) * O5</f>
-        <v>3000</v>
+        <f t="shared" si="1"/>
+        <v>2800</v>
       </c>
       <c r="G5" s="5">
         <f>(ROUND(B5/Parameters!B$15, 0) + 1)</f>
         <v>1</v>
       </c>
       <c r="H5" s="5" t="str">
-        <f t="shared" ref="H5" si="10">IF(J5&lt;=1024,"G.025X",IF(J5&lt;=2048,"G.1X", "G.2X"))</f>
+        <f t="shared" ref="H5" si="9">IF(J5&lt;=1024,"G.025X",IF(J5&lt;=2048,"G.1X", "G.2X"))</f>
         <v>G.1X</v>
       </c>
       <c r="I5" s="4" t="s">
@@ -1110,11 +1110,11 @@
         <v>70</v>
       </c>
       <c r="L5" s="5">
-        <f t="shared" ref="L5" si="11">ROUNDUP(N5+O5,0)</f>
+        <f t="shared" ref="L5" si="10">ROUNDUP(N5+O5,0)</f>
         <v>4</v>
       </c>
       <c r="M5" s="7">
-        <f t="shared" ref="M5" si="12">((B5 * 1.6) * 1024 * 1024 ) / ROUNDUP(J5 / 1024, 0)</f>
+        <f t="shared" ref="M5" si="11">((B5 * 1.6) * 1024 * 1024 ) / ROUNDUP(J5 / 1024, 0)</f>
         <v>9227468.8000000007</v>
       </c>
       <c r="N5" s="5">
@@ -1122,11 +1122,11 @@
         <v>2</v>
       </c>
       <c r="O5" s="5">
-        <f t="shared" ref="O5" si="13">((ROUNDUP((M5) / R5,0) + 1)/IF(H5="G.025X",4,IF(H5="G.1X",1,IF(H5="G.2X",0.5))) * G5)</f>
+        <f t="shared" ref="O5" si="12">((ROUNDUP((M5) / R5,0) + 1)/IF(H5="G.025X",4,IF(H5="G.1X",1,IF(H5="G.2X",0.5))) * G5)</f>
         <v>2</v>
       </c>
       <c r="P5" s="5">
-        <f t="shared" ref="P5" si="14">N5+O5</f>
+        <f t="shared" ref="P5" si="13">N5+O5</f>
         <v>4</v>
       </c>
       <c r="Q5" s="8">
@@ -1134,7 +1134,7 @@
         <v>2</v>
       </c>
       <c r="R5" s="8">
-        <f t="shared" ref="R5" si="15">IF(H5 = "G.025X", 8000000, IF(H5= "G.1X", 16000000, IF(H5= "G.2X", 32000000)))</f>
+        <f t="shared" ref="R5" si="14">IF(H5 = "G.025X", 8000000, IF(H5= "G.1X", 16000000, IF(H5= "G.2X", 32000000)))</f>
         <v>16000000</v>
       </c>
     </row>
@@ -1165,7 +1165,7 @@
       </c>
       <c r="F6" s="5">
         <f t="shared" si="1"/>
-        <v>24000</v>
+        <v>22400</v>
       </c>
       <c r="G6" s="5">
         <f>(ROUND(B6/Parameters!B$15, 0) + 1)</f>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="Q6" s="8">
         <f>ROUNDUP(((C6 * 1024 * 1024) / F6) / 3600, 0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R6" s="8">
         <f t="shared" si="7"/>
@@ -1478,7 +1478,7 @@
       </c>
       <c r="B2" s="5">
         <f>SUM('List of artifacts'!F2:F6)*(B7/100+1)</f>
-        <v>290193.75</v>
+        <v>150123.75</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>13</v>
@@ -1502,7 +1502,7 @@
       </c>
       <c r="B4" s="5">
         <f>SUM('List of artifacts'!Q2:Q6)*(B7/100+1)</f>
-        <v>9.4500000000000011</v>
+        <v>14.700000000000001</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>62</v>
@@ -1526,7 +1526,7 @@
       </c>
       <c r="B6" s="5">
         <f>(B4*Parameters!B13*B5)*(B7/100+1)</f>
-        <v>1634.2655175</v>
+        <v>2542.1908050000002</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>36</v>

</xml_diff>